<commit_message>
update figure 1 in M2.1b
</commit_message>
<xml_diff>
--- a/IO_M2.1_new/M2.1b_outputs/M2.1b_Table1.xlsx
+++ b/IO_M2.1_new/M2.1b_outputs/M2.1b_Table1.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="258">
   <si>
     <t>runname</t>
   </si>
@@ -853,6 +853,12 @@
     <t>Assumed return
 (Discount rate)</t>
   </si>
+  <si>
+    <t>Note: 
+1. All values are percentage (%).
+2. These are simulated scenarios that are intended to reflect main features of investment practices in certian return environments, they are not directly based on historical data. 
+3. It is assumed that all portfolios have the same Sharpe ratio of 0.46, and the Sharpe ratio does not change across risk-free rate regimes</t>
+  </si>
 </sst>
 </file>
 
@@ -1651,11 +1657,11 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="7" fillId="13" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="13" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="13" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="13" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2977,7 +2983,7 @@
   <dimension ref="A2:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3028,11 +3034,11 @@
     <row r="5" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="45"/>
       <c r="B5" s="45"/>
-      <c r="C5" s="208"/>
-      <c r="D5" s="208"/>
-      <c r="E5" s="208"/>
-      <c r="F5" s="208"/>
-      <c r="G5" s="208"/>
+      <c r="C5" s="207"/>
+      <c r="D5" s="207"/>
+      <c r="E5" s="207"/>
+      <c r="F5" s="207"/>
+      <c r="G5" s="207"/>
       <c r="H5" s="45"/>
       <c r="I5" s="45"/>
       <c r="J5" s="45"/>
@@ -3126,13 +3132,13 @@
     <row r="10" spans="1:10" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="45"/>
       <c r="B10" s="45"/>
-      <c r="C10" s="207" t="s">
-        <v>254</v>
-      </c>
-      <c r="D10" s="207"/>
-      <c r="E10" s="207"/>
-      <c r="F10" s="207"/>
-      <c r="G10" s="207"/>
+      <c r="C10" s="208" t="s">
+        <v>257</v>
+      </c>
+      <c r="D10" s="208"/>
+      <c r="E10" s="208"/>
+      <c r="F10" s="208"/>
+      <c r="G10" s="208"/>
       <c r="H10" s="45"/>
       <c r="I10" s="45"/>
       <c r="J10" s="45"/>
@@ -3296,14 +3302,14 @@
       <c r="L3" s="179"/>
       <c r="M3" s="179"/>
       <c r="O3" s="45"/>
-      <c r="P3" s="208" t="s">
+      <c r="P3" s="207" t="s">
         <v>246</v>
       </c>
-      <c r="Q3" s="208"/>
-      <c r="R3" s="208"/>
-      <c r="S3" s="208"/>
-      <c r="T3" s="208"/>
-      <c r="U3" s="208"/>
+      <c r="Q3" s="207"/>
+      <c r="R3" s="207"/>
+      <c r="S3" s="207"/>
+      <c r="T3" s="207"/>
+      <c r="U3" s="207"/>
       <c r="V3" s="45"/>
     </row>
     <row r="4" spans="3:22" ht="45" x14ac:dyDescent="0.25">
@@ -3630,14 +3636,14 @@
       <c r="L10" s="180"/>
       <c r="M10" s="180"/>
       <c r="O10" s="45"/>
-      <c r="P10" s="207" t="s">
+      <c r="P10" s="208" t="s">
         <v>245</v>
       </c>
-      <c r="Q10" s="207"/>
-      <c r="R10" s="207"/>
-      <c r="S10" s="207"/>
-      <c r="T10" s="207"/>
-      <c r="U10" s="207"/>
+      <c r="Q10" s="208"/>
+      <c r="R10" s="208"/>
+      <c r="S10" s="208"/>
+      <c r="T10" s="208"/>
+      <c r="U10" s="208"/>
       <c r="V10" s="45"/>
     </row>
     <row r="12" spans="3:22" x14ac:dyDescent="0.25">
@@ -7891,23 +7897,23 @@
     </row>
     <row r="5" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="45"/>
-      <c r="B5" s="208" t="s">
+      <c r="B5" s="207" t="s">
         <v>136</v>
       </c>
-      <c r="C5" s="208"/>
-      <c r="D5" s="208"/>
-      <c r="E5" s="208"/>
-      <c r="F5" s="208"/>
-      <c r="G5" s="208"/>
+      <c r="C5" s="207"/>
+      <c r="D5" s="207"/>
+      <c r="E5" s="207"/>
+      <c r="F5" s="207"/>
+      <c r="G5" s="207"/>
       <c r="H5" s="45"/>
       <c r="I5" s="45"/>
       <c r="J5" s="45"/>
       <c r="K5" s="45"/>
-      <c r="L5" s="208"/>
-      <c r="M5" s="208"/>
-      <c r="N5" s="208"/>
-      <c r="O5" s="208"/>
-      <c r="P5" s="208"/>
+      <c r="L5" s="207"/>
+      <c r="M5" s="207"/>
+      <c r="N5" s="207"/>
+      <c r="O5" s="207"/>
+      <c r="P5" s="207"/>
       <c r="Q5" s="45"/>
       <c r="R5" s="45"/>
       <c r="S5" s="45"/>
@@ -8083,25 +8089,25 @@
     </row>
     <row r="10" spans="1:19" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="45"/>
-      <c r="B10" s="207" t="s">
+      <c r="B10" s="208" t="s">
         <v>254</v>
       </c>
-      <c r="C10" s="207"/>
-      <c r="D10" s="207"/>
-      <c r="E10" s="207"/>
-      <c r="F10" s="207"/>
-      <c r="G10" s="207"/>
+      <c r="C10" s="208"/>
+      <c r="D10" s="208"/>
+      <c r="E10" s="208"/>
+      <c r="F10" s="208"/>
+      <c r="G10" s="208"/>
       <c r="H10" s="45"/>
       <c r="I10" s="45"/>
       <c r="J10" s="45"/>
       <c r="K10" s="45"/>
-      <c r="L10" s="207" t="s">
+      <c r="L10" s="208" t="s">
         <v>254</v>
       </c>
-      <c r="M10" s="207"/>
-      <c r="N10" s="207"/>
-      <c r="O10" s="207"/>
-      <c r="P10" s="207"/>
+      <c r="M10" s="208"/>
+      <c r="N10" s="208"/>
+      <c r="O10" s="208"/>
+      <c r="P10" s="208"/>
       <c r="Q10" s="45"/>
       <c r="R10" s="45"/>
       <c r="S10" s="45"/>
@@ -36944,7 +36950,7 @@
   <sheetData>
     <row r="6" spans="1:16" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="45"/>
-      <c r="B6" s="208" t="s">
+      <c r="B6" s="207" t="s">
         <v>136</v>
       </c>
       <c r="C6" s="209"/>
@@ -37396,11 +37402,11 @@
   <sheetData>
     <row r="3" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="45"/>
-      <c r="C3" s="208" t="s">
+      <c r="C3" s="207" t="s">
         <v>136</v>
       </c>
-      <c r="D3" s="208"/>
-      <c r="E3" s="208"/>
+      <c r="D3" s="207"/>
+      <c r="E3" s="207"/>
       <c r="F3" s="209"/>
       <c r="G3" s="209"/>
       <c r="H3" s="209"/>

</xml_diff>